<commit_message>
looks like guru99 v3 can't delete created customers yet , they only shoving alert, that's why we need to refresh exel file before run or test fails because app does'n add existing customer
</commit_message>
<xml_diff>
--- a/src/main/resources/customers.xlsx
+++ b/src/main/resources/customers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dima\Desktop\TestngProject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E46D789-A395-45CA-BEA9-119FE7C600D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B02F534-B3CB-4A8B-AB06-1CB6F208FD85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5064" yWindow="1680" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Customers1" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>alexis</t>
-  </si>
-  <si>
     <t>f</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>"12345678"</t>
   </si>
   <si>
-    <t>Dina</t>
-  </si>
-  <si>
     <t>"05102001</t>
   </si>
   <si>
@@ -90,22 +84,28 @@
     <t>WS</t>
   </si>
   <si>
-    <t>"000000"</t>
-  </si>
-  <si>
     <t>"054321111112231"</t>
   </si>
   <si>
     <t>"054321111112232"</t>
   </si>
   <si>
-    <t>"111123"</t>
-  </si>
-  <si>
-    <t>stsADDd+Din@gmail.com</t>
-  </si>
-  <si>
-    <t>artahaststAlsd+1@gmail.com</t>
+    <t>"222222"</t>
+  </si>
+  <si>
+    <t>"333333"</t>
+  </si>
+  <si>
+    <t>alexiss</t>
+  </si>
+  <si>
+    <t>Dinas</t>
+  </si>
+  <si>
+    <t>artahAlsd+1@gmail.com</t>
+  </si>
+  <si>
+    <t>stsADDdDN+Din@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,8 +445,8 @@
     <col min="3" max="3" width="11" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="9.88671875" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="21.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" customWidth="1"/>
     <col min="10" max="10" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -484,66 +484,66 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>23</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>